<commit_message>
Revert "Merge branch 'master' of https://github.com/duyot/WMS into update_goods_infor" update This reverts commit 8d51d69a1546afc32cdd6d2e37523b54d99f453f, reversing  e007c3771e3105d98cc62d4073ddf79275a0359e. revert commit
</commit_message>
<xml_diff>
--- a/Document/0.PM/ChiPhi.xlsx
+++ b/Document/0.PM/ChiPhi.xlsx
@@ -1,18 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA0B17F-E49F-45BA-A2A8-1A86B3166AEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5886D2-434E-4C50-8A22-1700E4E7A3DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$G$17</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>TT</t>
   </si>
@@ -81,62 +78,10 @@
     <t>Mua domain logdez.com 2 năm</t>
   </si>
   <si>
+    <t>15.77USD/tháng</t>
+  </si>
+  <si>
     <t>Chi phí host tháng 6/2019</t>
-  </si>
-  <si>
-    <t>Chi phí thành lập doanh nghiệp</t>
-  </si>
-  <si>
-    <t>Chi phí mua biển công ty</t>
-  </si>
-  <si>
-    <t>Chi phí mua token key</t>
-  </si>
-  <si>
-    <t>3 năm</t>
-  </si>
-  <si>
-    <t>Chỉ phải nộp nửa năm do thành lập từ 24/7</t>
-  </si>
-  <si>
-    <t>25/7/2019</t>
-  </si>
-  <si>
-    <t>DuyOT
-DoanLV4</t>
-  </si>
-  <si>
-    <t>Chi cục thuế kiểm tra</t>
-  </si>
-  <si>
-    <t>Chi phí host tháng 7/2019</t>
-  </si>
-  <si>
-    <t>Chi phí mua hóa đơn điện tử (300 đơn)</t>
-  </si>
-  <si>
-    <t>22/8/2019</t>
-  </si>
-  <si>
-    <t>Nhóm</t>
-  </si>
-  <si>
-    <t>Host</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>Setup Company</t>
-  </si>
-  <si>
-    <t>Nộp thuế muôn bài</t>
-  </si>
-  <si>
-    <t>15 USD/tháng</t>
-  </si>
-  <si>
-    <t>Chi phí host tháng 8/2019</t>
   </si>
 </sst>
 </file>
@@ -205,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -226,19 +171,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -583,50 +515,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="33.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" customWidth="1"/>
-    <col min="7" max="7" width="43.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.6328125" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="43.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F3" s="5">
-        <f>SUM(F5:F254)</f>
-        <v>11119000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E3" s="5">
+        <f>SUM(E5:E254)</f>
+        <v>4189000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -634,22 +563,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -657,22 +583,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2">
+      <c r="E5" s="2">
         <v>1200000</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -680,20 +603,17 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8">
+      <c r="D6" s="8">
         <v>43215</v>
       </c>
-      <c r="F6" s="2">
+      <c r="E6" s="2">
         <v>200000</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -701,21 +621,18 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2">
+      <c r="D7" s="1"/>
+      <c r="E7" s="2">
         <f>5*12*23000</f>
         <v>1380000</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -723,22 +640,19 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="8">
+      <c r="D8" s="8">
         <v>43501</v>
       </c>
-      <c r="F8" s="9">
+      <c r="E8" s="9">
         <v>365000</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -746,22 +660,19 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="8">
+      <c r="D9" s="8">
         <v>43502</v>
       </c>
-      <c r="F9" s="9">
+      <c r="E9" s="9">
         <v>365000</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -769,203 +680,69 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="8">
+      <c r="D10" s="8">
         <v>43502</v>
       </c>
-      <c r="F10" s="9">
+      <c r="E10" s="9">
         <v>314000</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>7</v>
-      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8">
+        <v>43502</v>
+      </c>
+      <c r="E11" s="9">
+        <v>365000</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="8">
-        <v>43503</v>
-      </c>
-      <c r="F11" s="9">
-        <v>365000</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="9">
-        <v>2000000</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="9">
-        <v>200000</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="9">
-        <v>1500000</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="9">
-        <v>1000000</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="13">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="8">
-        <v>43473</v>
-      </c>
-      <c r="F16" s="9">
-        <v>365000</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="13">
-        <v>13</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="14">
-        <v>1500000</v>
-      </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="13">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="8">
-        <v>43474</v>
-      </c>
-      <c r="F18" s="9">
-        <v>365000</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>35</v>
-      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:G17" xr:uid="{3C114EBF-F9B7-4C6E-B13B-77DBBA155778}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>